<commit_message>
major update to inventory clean up script. made a new inventory spatial clean up (01) script
</commit_message>
<xml_diff>
--- a/scripts/Provincial_Tools/tbl_sql_classify.xlsx
+++ b/scripts/Provincial_Tools/tbl_sql_classify.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F511C28C-C833-43CF-91A4-6364C1E39BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3996486-FC43-4D1A-86A0-767E4F9DE686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tbl_sql_classify" sheetId="2" r:id="rId1"/>
-    <sheet name="tbl_sql_classify_originalLW" sheetId="1" r:id="rId2"/>
+    <sheet name="Instruction" sheetId="3" r:id="rId1"/>
+    <sheet name="tbl_sql_classify" sheetId="2" r:id="rId2"/>
+    <sheet name="tbl_sql_classify_originalLW" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="tbl_sql_classify" localSheetId="0">tbl_sql_classify!$A$1:$F$482</definedName>
+    <definedName name="tbl_sql_classify" localSheetId="1">tbl_sql_classify!$A$1:$F$482</definedName>
     <definedName name="tbl_sql_classify">tbl_sql_classify_originalLW!$A$1:$F$481</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3930" uniqueCount="631">
   <si>
     <t>RECNO</t>
   </si>
@@ -1955,6 +1956,9 @@
   </si>
   <si>
     <t>POLYTYPE='FOR'</t>
+  </si>
+  <si>
+    <t>Careful when using 'NA'. some scripts automatically change this to 'nan'</t>
   </si>
 </sst>
 </file>
@@ -2017,6 +2021,108 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0849585B-161F-511B-1D0E-C8B848B8A501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="819150" y="304800"/>
+          <a:ext cx="5876925" cy="2828925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>This workbook</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> is related to the tool PIAM02 Populate Econum SFU PFT LGFU.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Any changes made on this xlsx doesn't impact</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> the tool unless you export this as csv file.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>It's highly recommended not to edit this file unless you are certain something is off.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Kim, Daniel (MNR)" id="{264968DA-A092-4D89-A15E-5FC7711A2087}" userId="S::Daniel.Kim2@ontario.ca::6a941af3-110c-4c3c-b425-309817122f3e" providerId="AD"/>
@@ -2025,13 +2131,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78662066-8961-40A1-8222-90158F51F698}" name="Table2" displayName="Table2" ref="A1:I482" totalsRowShown="0">
-  <autoFilter ref="A1:I482" xr:uid="{78662066-8961-40A1-8222-90158F51F698}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="NEBOR"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I482" xr:uid="{78662066-8961-40A1-8222-90158F51F698}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A0EAC60B-668E-44A3-9B0D-478FBC6B6047}" name="RECNO"/>
     <tableColumn id="2" xr3:uid="{FF83C207-30F8-4195-90E0-902ED8E62390}" name="REGION"/>
@@ -2365,21 +2465,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75554A27-DDC8-4041-BCB3-C891473CBC18}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD4AE21-1701-4E7D-951A-9CFF25966ACE}">
   <dimension ref="A1:I482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B161" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="65.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="124.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="75.28515625" customWidth="1"/>
@@ -2414,7 +2527,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2437,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2460,7 +2573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2483,7 +2596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2506,7 +2619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2526,7 +2639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2546,7 +2659,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2566,7 +2679,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2586,7 +2699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2606,7 +2719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2626,7 +2739,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2646,7 +2759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2666,7 +2779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2686,7 +2799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2706,7 +2819,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2726,7 +2839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2746,7 +2859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2766,7 +2879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2786,7 +2899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2806,7 +2919,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2826,7 +2939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2846,7 +2959,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2866,7 +2979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2886,7 +2999,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2906,7 +3019,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2926,7 +3039,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2946,7 +3059,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2966,7 +3079,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2986,7 +3099,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3006,7 +3119,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3026,7 +3139,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3046,7 +3159,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3066,7 +3179,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3086,7 +3199,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3106,7 +3219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3126,7 +3239,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3146,7 +3259,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3166,7 +3279,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3186,7 +3299,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3206,7 +3319,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3226,7 +3339,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3246,7 +3359,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3266,7 +3379,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3286,7 +3399,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3306,7 +3419,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3326,7 +3439,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3346,7 +3459,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3366,7 +3479,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3386,7 +3499,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3406,7 +3519,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3426,7 +3539,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3446,7 +3559,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3466,7 +3579,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3486,7 +3599,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3506,7 +3619,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3526,7 +3639,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3546,7 +3659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3566,7 +3679,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3586,7 +3699,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3606,7 +3719,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3626,7 +3739,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3646,7 +3759,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3666,7 +3779,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3686,7 +3799,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3706,7 +3819,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3726,7 +3839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3746,7 +3859,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3766,7 +3879,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3786,7 +3899,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3806,7 +3919,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3826,7 +3939,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3846,7 +3959,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3866,7 +3979,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3886,7 +3999,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3906,7 +4019,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3926,7 +4039,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3946,7 +4059,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3966,7 +4079,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3986,7 +4099,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4006,7 +4119,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4026,7 +4139,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4046,7 +4159,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4066,7 +4179,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4086,7 +4199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4106,7 +4219,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4126,7 +4239,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4146,7 +4259,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4166,7 +4279,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4186,7 +4299,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4206,7 +4319,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4226,7 +4339,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4246,7 +4359,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4266,7 +4379,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4286,7 +4399,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4306,7 +4419,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4326,7 +4439,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4346,7 +4459,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4366,7 +4479,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4386,7 +4499,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4406,7 +4519,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4426,7 +4539,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4446,7 +4559,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4466,7 +4579,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4486,7 +4599,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4506,7 +4619,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4526,7 +4639,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4546,7 +4659,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4566,7 +4679,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4586,7 +4699,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4606,7 +4719,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4626,7 +4739,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4646,7 +4759,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4666,7 +4779,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4686,7 +4799,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4706,7 +4819,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4726,7 +4839,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4746,7 +4859,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4766,7 +4879,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4786,7 +4899,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4806,7 +4919,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4826,7 +4939,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4846,7 +4959,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4866,7 +4979,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4886,7 +4999,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4906,7 +5019,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4926,7 +5039,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4946,7 +5059,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4966,7 +5079,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4986,7 +5099,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5006,7 +5119,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5026,7 +5139,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5046,7 +5159,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5066,7 +5179,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5086,7 +5199,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5106,7 +5219,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5126,7 +5239,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5146,7 +5259,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5166,7 +5279,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5186,7 +5299,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5206,7 +5319,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5226,7 +5339,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5246,7 +5359,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5377,6 +5490,9 @@
       <c r="F148" t="s">
         <v>17</v>
       </c>
+      <c r="I148" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
@@ -8218,7 +8334,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>600</v>
       </c>
@@ -8238,7 +8354,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>601</v>
       </c>
@@ -8258,7 +8374,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>602</v>
       </c>
@@ -8278,7 +8394,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>603</v>
       </c>
@@ -8298,7 +8414,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>604</v>
       </c>
@@ -8318,7 +8434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>610</v>
       </c>
@@ -8338,7 +8454,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>611</v>
       </c>
@@ -8358,7 +8474,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="289" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>612</v>
       </c>
@@ -8378,7 +8494,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>613</v>
       </c>
@@ -8398,7 +8514,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="291" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>614</v>
       </c>
@@ -8418,7 +8534,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="292" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>615</v>
       </c>
@@ -8438,7 +8554,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="293" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>616</v>
       </c>
@@ -8458,7 +8574,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="294" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>617</v>
       </c>
@@ -8478,7 +8594,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="295" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>618</v>
       </c>
@@ -8498,7 +8614,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="296" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>619</v>
       </c>
@@ -8518,7 +8634,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>620</v>
       </c>
@@ -8538,7 +8654,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>621</v>
       </c>
@@ -8558,7 +8674,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>622</v>
       </c>
@@ -8578,7 +8694,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>623</v>
       </c>
@@ -8598,7 +8714,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>624</v>
       </c>
@@ -8618,7 +8734,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>625</v>
       </c>
@@ -8638,7 +8754,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>626</v>
       </c>
@@ -8658,7 +8774,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>627</v>
       </c>
@@ -8678,7 +8794,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>628</v>
       </c>
@@ -8698,7 +8814,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>629</v>
       </c>
@@ -8718,7 +8834,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>630</v>
       </c>
@@ -8738,7 +8854,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>631</v>
       </c>
@@ -8758,7 +8874,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>632</v>
       </c>
@@ -8778,7 +8894,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>633</v>
       </c>
@@ -8798,7 +8914,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>634</v>
       </c>
@@ -8818,7 +8934,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>635</v>
       </c>
@@ -8838,7 +8954,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>636</v>
       </c>
@@ -8858,7 +8974,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>640</v>
       </c>
@@ -8878,7 +8994,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>641</v>
       </c>
@@ -8898,7 +9014,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>642</v>
       </c>
@@ -8918,7 +9034,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>643</v>
       </c>
@@ -8938,7 +9054,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>644</v>
       </c>
@@ -8958,7 +9074,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>645</v>
       </c>
@@ -8978,7 +9094,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>646</v>
       </c>
@@ -8998,7 +9114,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>647</v>
       </c>
@@ -9018,7 +9134,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>650</v>
       </c>
@@ -9038,7 +9154,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>651</v>
       </c>
@@ -9058,7 +9174,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>652</v>
       </c>
@@ -9078,7 +9194,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>653</v>
       </c>
@@ -9098,7 +9214,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>654</v>
       </c>
@@ -9118,7 +9234,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>655</v>
       </c>
@@ -9138,7 +9254,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>656</v>
       </c>
@@ -9158,7 +9274,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>657</v>
       </c>
@@ -9178,7 +9294,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>658</v>
       </c>
@@ -9198,7 +9314,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>659</v>
       </c>
@@ -9218,7 +9334,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>660</v>
       </c>
@@ -9238,7 +9354,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>661</v>
       </c>
@@ -9258,7 +9374,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>662</v>
       </c>
@@ -9278,7 +9394,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>663</v>
       </c>
@@ -9298,7 +9414,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>664</v>
       </c>
@@ -9318,7 +9434,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>665</v>
       </c>
@@ -9338,7 +9454,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>666</v>
       </c>
@@ -9358,7 +9474,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>667</v>
       </c>
@@ -9378,7 +9494,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>668</v>
       </c>
@@ -9398,7 +9514,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>669</v>
       </c>
@@ -9418,7 +9534,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>670</v>
       </c>
@@ -9438,7 +9554,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>671</v>
       </c>
@@ -9458,7 +9574,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>672</v>
       </c>
@@ -9478,7 +9594,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>673</v>
       </c>
@@ -9498,7 +9614,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>674</v>
       </c>
@@ -9518,7 +9634,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>675</v>
       </c>
@@ -9538,7 +9654,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>676</v>
       </c>
@@ -9558,7 +9674,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>680</v>
       </c>
@@ -9578,7 +9694,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>681</v>
       </c>
@@ -9598,7 +9714,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>682</v>
       </c>
@@ -9618,7 +9734,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>683</v>
       </c>
@@ -9638,7 +9754,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>684</v>
       </c>
@@ -9658,7 +9774,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>685</v>
       </c>
@@ -9678,7 +9794,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>686</v>
       </c>
@@ -9698,7 +9814,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>687</v>
       </c>
@@ -9718,7 +9834,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>688</v>
       </c>
@@ -9738,7 +9854,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>689</v>
       </c>
@@ -9758,7 +9874,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>690</v>
       </c>
@@ -9778,7 +9894,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>691</v>
       </c>
@@ -9798,7 +9914,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>692</v>
       </c>
@@ -9818,7 +9934,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>693</v>
       </c>
@@ -9838,7 +9954,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>694</v>
       </c>
@@ -9858,7 +9974,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>695</v>
       </c>
@@ -9878,7 +9994,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>696</v>
       </c>
@@ -9898,7 +10014,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>697</v>
       </c>
@@ -9918,7 +10034,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>698</v>
       </c>
@@ -9938,7 +10054,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>699</v>
       </c>
@@ -9958,7 +10074,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>700</v>
       </c>
@@ -9978,7 +10094,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>701</v>
       </c>
@@ -9998,7 +10114,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>702</v>
       </c>
@@ -10018,7 +10134,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>703</v>
       </c>
@@ -10038,7 +10154,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>704</v>
       </c>
@@ -10058,7 +10174,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>705</v>
       </c>
@@ -10078,7 +10194,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>706</v>
       </c>
@@ -10098,7 +10214,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>707</v>
       </c>
@@ -10118,7 +10234,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>708</v>
       </c>
@@ -10138,7 +10254,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>709</v>
       </c>
@@ -10158,7 +10274,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>710</v>
       </c>
@@ -10178,7 +10294,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>711</v>
       </c>
@@ -10198,7 +10314,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>712</v>
       </c>
@@ -10218,7 +10334,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>713</v>
       </c>
@@ -10238,7 +10354,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>714</v>
       </c>
@@ -10258,7 +10374,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>715</v>
       </c>
@@ -10278,7 +10394,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>716</v>
       </c>
@@ -10298,7 +10414,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>717</v>
       </c>
@@ -10318,7 +10434,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>718</v>
       </c>
@@ -10338,7 +10454,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>719</v>
       </c>
@@ -10358,7 +10474,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>720</v>
       </c>
@@ -10378,7 +10494,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>721</v>
       </c>
@@ -10398,7 +10514,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>722</v>
       </c>
@@ -10418,7 +10534,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>723</v>
       </c>
@@ -10438,7 +10554,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>724</v>
       </c>
@@ -10458,7 +10574,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>725</v>
       </c>
@@ -10478,7 +10594,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>726</v>
       </c>
@@ -10498,7 +10614,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>727</v>
       </c>
@@ -10518,7 +10634,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>728</v>
       </c>
@@ -10538,7 +10654,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>729</v>
       </c>
@@ -10558,7 +10674,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>730</v>
       </c>
@@ -10578,7 +10694,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>731</v>
       </c>
@@ -10598,7 +10714,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>732</v>
       </c>
@@ -10618,7 +10734,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>733</v>
       </c>
@@ -10638,7 +10754,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>734</v>
       </c>
@@ -10658,7 +10774,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>735</v>
       </c>
@@ -10678,7 +10794,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>736</v>
       </c>
@@ -10698,7 +10814,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>737</v>
       </c>
@@ -10718,7 +10834,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>738</v>
       </c>
@@ -10738,7 +10854,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>739</v>
       </c>
@@ -10758,7 +10874,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="409" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>740</v>
       </c>
@@ -10778,7 +10894,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="410" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>741</v>
       </c>
@@ -10798,7 +10914,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="411" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>742</v>
       </c>
@@ -10818,7 +10934,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="412" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>743</v>
       </c>
@@ -10838,7 +10954,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="413" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>744</v>
       </c>
@@ -10858,7 +10974,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="414" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>745</v>
       </c>
@@ -10878,7 +10994,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="415" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>746</v>
       </c>
@@ -10898,7 +11014,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="416" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>747</v>
       </c>
@@ -10918,7 +11034,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="417" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>748</v>
       </c>
@@ -10938,7 +11054,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="418" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>749</v>
       </c>
@@ -10958,7 +11074,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="419" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>750</v>
       </c>
@@ -10978,7 +11094,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="420" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>751</v>
       </c>
@@ -10998,7 +11114,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>752</v>
       </c>
@@ -11018,7 +11134,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="422" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>753</v>
       </c>
@@ -11038,7 +11154,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="423" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>754</v>
       </c>
@@ -11058,7 +11174,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="424" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>755</v>
       </c>
@@ -11078,7 +11194,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="425" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>756</v>
       </c>
@@ -11098,7 +11214,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="426" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>757</v>
       </c>
@@ -11118,7 +11234,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="427" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>758</v>
       </c>
@@ -11138,7 +11254,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="428" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>759</v>
       </c>
@@ -11158,7 +11274,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="429" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>760</v>
       </c>
@@ -11178,7 +11294,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="430" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>761</v>
       </c>
@@ -11198,7 +11314,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="431" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>762</v>
       </c>
@@ -11218,7 +11334,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="432" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>763</v>
       </c>
@@ -11238,7 +11354,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="433" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>764</v>
       </c>
@@ -11258,7 +11374,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="434" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>765</v>
       </c>
@@ -11278,7 +11394,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="435" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>766</v>
       </c>
@@ -11298,7 +11414,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="436" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>767</v>
       </c>
@@ -11318,7 +11434,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="437" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>768</v>
       </c>
@@ -11338,7 +11454,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="438" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>769</v>
       </c>
@@ -11358,7 +11474,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="439" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>770</v>
       </c>
@@ -11378,7 +11494,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="440" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>771</v>
       </c>
@@ -11398,7 +11514,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="441" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>772</v>
       </c>
@@ -11418,7 +11534,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="442" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>773</v>
       </c>
@@ -11438,7 +11554,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="443" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>774</v>
       </c>
@@ -11458,7 +11574,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="444" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>775</v>
       </c>
@@ -11478,7 +11594,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="445" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>776</v>
       </c>
@@ -11498,7 +11614,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="446" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>777</v>
       </c>
@@ -11518,7 +11634,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>778</v>
       </c>
@@ -11538,7 +11654,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="448" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>779</v>
       </c>
@@ -11558,7 +11674,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="449" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>780</v>
       </c>
@@ -11578,7 +11694,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="450" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>781</v>
       </c>
@@ -11598,7 +11714,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="451" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>782</v>
       </c>
@@ -11618,7 +11734,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="452" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>783</v>
       </c>
@@ -11638,7 +11754,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="453" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>784</v>
       </c>
@@ -11658,7 +11774,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="454" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>785</v>
       </c>
@@ -11678,7 +11794,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="455" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>786</v>
       </c>
@@ -11698,7 +11814,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="456" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>787</v>
       </c>
@@ -11718,7 +11834,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="457" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>788</v>
       </c>
@@ -11738,7 +11854,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="458" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>789</v>
       </c>
@@ -11758,7 +11874,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="459" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>790</v>
       </c>
@@ -11778,7 +11894,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="460" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>791</v>
       </c>
@@ -11798,7 +11914,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="461" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>792</v>
       </c>
@@ -11818,7 +11934,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="462" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>793</v>
       </c>
@@ -11838,7 +11954,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="463" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>794</v>
       </c>
@@ -11858,7 +11974,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="464" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>795</v>
       </c>
@@ -11878,7 +11994,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="465" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>796</v>
       </c>
@@ -11898,7 +12014,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="466" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>797</v>
       </c>
@@ -11918,7 +12034,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="467" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>798</v>
       </c>
@@ -11938,7 +12054,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="468" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>799</v>
       </c>
@@ -11958,7 +12074,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="469" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>800</v>
       </c>
@@ -11978,7 +12094,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="470" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>801</v>
       </c>
@@ -11998,7 +12114,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="471" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>802</v>
       </c>
@@ -12018,7 +12134,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="472" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>803</v>
       </c>
@@ -12038,7 +12154,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="473" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>804</v>
       </c>
@@ -12058,7 +12174,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="474" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>805</v>
       </c>
@@ -12078,7 +12194,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="475" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>810</v>
       </c>
@@ -12098,7 +12214,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="476" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>811</v>
       </c>
@@ -12118,7 +12234,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="477" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>812</v>
       </c>
@@ -12138,7 +12254,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="478" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>813</v>
       </c>
@@ -12158,7 +12274,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="479" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>814</v>
       </c>
@@ -12178,7 +12294,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="480" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>815</v>
       </c>
@@ -12198,7 +12314,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="481" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>816</v>
       </c>
@@ -12218,7 +12334,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="482" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>817</v>
       </c>
@@ -12248,7 +12364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>

</xml_diff>

<commit_message>
major edits to tbl_sql_classify.csv - especially PO1, POSHA, PODEE and BW
</commit_message>
<xml_diff>
--- a/scripts/Provincial_Tools/tbl_sql_classify.xlsx
+++ b/scripts/Provincial_Tools/tbl_sql_classify.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3996486-FC43-4D1A-86A0-767E4F9DE686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE9A450-392E-44BD-A8D2-3745384C39D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="3" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3930" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3956" uniqueCount="654">
   <si>
     <t>RECNO</t>
   </si>
@@ -1904,9 +1904,6 @@
     <t>PO+PT+PL+BW+MH+YB+MR+AB+EX+PB&gt;=70 AND PO+PT+PL+PB&gt;=50</t>
   </si>
   <si>
-    <t>PO+BW+YB+MR+UH+MH+LH+OH&gt;=70</t>
-  </si>
-  <si>
     <t>(BF&lt;=20 AND SW&lt;=20 AND CE&lt;=20 AND PO+PT+PL+BW+MH+YB+MR+AB+EX+PB&gt;=50 AND PJ+PR&lt;=50 AND PJ+PR&gt;=20 AND ECONUM IN (16,19,28,40,43,55,59,70,76))</t>
   </si>
   <si>
@@ -1959,6 +1956,78 @@
   </si>
   <si>
     <t>Careful when using 'NA'. some scripts automatically change this to 'nan'</t>
+  </si>
+  <si>
+    <t>originally (Po &gt;= 70 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>originally (Po &gt;= 70)</t>
+  </si>
+  <si>
+    <t>originally (Bw &gt;= 60 And Po + Bw &gt;= 70 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>originally (Bw &gt;= 60 And Po + Bw &gt;= 70)</t>
+  </si>
+  <si>
+    <t>(PO+PT+PL &gt;= 70 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>(PO+PT+PL&gt;= 70)</t>
+  </si>
+  <si>
+    <t>confirmed with G. Beemer's SQL</t>
+  </si>
+  <si>
+    <t>originally (Ce + La &gt;= 50 Or (LeadSpc = 'Ce' or LeadSpc = 'La')) And EcoGrp = 'ConLow'</t>
+  </si>
+  <si>
+    <t>originally (EcoGrp = 'ConLow') Or (EcoGrp = 'HwdLow' And AllCon &gt; AllHwd)</t>
+  </si>
+  <si>
+    <t>originally (Sb &gt;= 70 And Po + Bw &lt;= 20)</t>
+  </si>
+  <si>
+    <t>originally (Pj &gt;= 70 And Po + Bw &lt;= 20 and EcoGrp='ShalES') Or (Pj &gt;= 50 And Po + Bw &lt;= 20 And AGE &gt;= 120 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>originally (Pj &gt;= 70 And Po + Bw &lt;= 20) Or (Pj &gt;= 50 And Po + Bw &lt;= 20 And AGE &gt;= 120) Or (Pj &gt;= 70 And (EcoNum = 34 or EcoNum = 35))</t>
+  </si>
+  <si>
+    <t>(Ce + La &gt;= 50 Or LEADSPC in ('CE','LA','CW')) And EcoGrp = 'ConLow'</t>
+  </si>
+  <si>
+    <t>revised with G. Beemer's SQL</t>
+  </si>
+  <si>
+    <t>(Sb &gt;= 70 And PO+PT+PL+ Bw &lt;= 20 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>(Sb &gt;= 70 And PO+PT+PL+ Bw &lt;= 20)</t>
+  </si>
+  <si>
+    <t>(Pj &gt;= 70 And PO+PT+PL+ Bw &lt;= 20 and EcoGrp='ShalES') Or (Pj &gt;= 50 And PO+PT+PL+ Bw &lt;= 20 And AGE &gt;= 120 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>(Bw &gt;= 60 And PO+PT+PL + Bw &gt;= 70 And EcoGrp = 'ShalES')</t>
+  </si>
+  <si>
+    <t>(Bw &gt;= 60 And PO+PT+PL + Bw &gt;= 70)</t>
+  </si>
+  <si>
+    <t>AllCon &gt;= 70 And Bf &lt;= 10 And PO+PT+PL + Bw &lt;= 20 And Sb + Sw &gt; Pj And Sb + Sw + Pj &gt;= 40</t>
+  </si>
+  <si>
+    <t>AllCon &gt;= 70 And Bf &lt;= 10 And PO+PT+PL + Bw &lt;= 20 And Sb + Sw &lt;= Pj And Sb + Sw + Pj &gt;= 40</t>
+  </si>
+  <si>
+    <t>(Pj &gt;= 70 And PO+PT+PL + Bw &lt;= 20) Or (Pj &gt;= 50 And PO+PT+PL + Bw &lt;= 20 And AGE &gt;= 120) Or (Pj &gt;= 70 And EcoNum in (34,35))</t>
+  </si>
+  <si>
+    <t>Larry used to group PO, PT, PL to PO. Now that they are separate, I must edit this script. Verified with G Beemer's SQL.</t>
+  </si>
+  <si>
+    <t>PO+PT+PL+BW+MH+YB+MR+AB+EX+PB&gt;=70</t>
   </si>
 </sst>
 </file>
@@ -2481,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD4AE21-1701-4E7D-951A-9CFF25966ACE}">
   <dimension ref="A1:I482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2562,7 @@
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="124.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="75.28515625" customWidth="1"/>
   </cols>
@@ -2544,7 +2613,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
@@ -2567,7 +2636,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
@@ -2590,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -2613,7 +2682,7 @@
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>15</v>
@@ -2658,6 +2727,9 @@
       <c r="F7" t="s">
         <v>20</v>
       </c>
+      <c r="I7" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2678,6 +2750,9 @@
       <c r="F8" t="s">
         <v>22</v>
       </c>
+      <c r="I8" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2698,6 +2773,9 @@
       <c r="F9" t="s">
         <v>24</v>
       </c>
+      <c r="I9" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2718,6 +2796,9 @@
       <c r="F10" t="s">
         <v>26</v>
       </c>
+      <c r="I10" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2736,7 +2817,13 @@
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>642</v>
+      </c>
+      <c r="H11" t="s">
+        <v>637</v>
+      </c>
+      <c r="I11" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2776,7 +2863,13 @@
         <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>644</v>
+      </c>
+      <c r="H13" t="s">
+        <v>638</v>
+      </c>
+      <c r="I13" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2796,7 +2889,13 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>645</v>
+      </c>
+      <c r="H14" t="s">
+        <v>639</v>
+      </c>
+      <c r="I14" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2816,7 +2915,13 @@
         <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>646</v>
+      </c>
+      <c r="H15" t="s">
+        <v>640</v>
+      </c>
+      <c r="I15" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2836,10 +2941,16 @@
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+      <c r="H16" t="s">
+        <v>641</v>
+      </c>
+      <c r="I16" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2856,10 +2967,16 @@
         <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+      <c r="H17" t="s">
+        <v>630</v>
+      </c>
+      <c r="I17" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2876,10 +2993,16 @@
         <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+      <c r="H18" t="s">
+        <v>631</v>
+      </c>
+      <c r="I18" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2896,10 +3019,16 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+      <c r="H19" t="s">
+        <v>632</v>
+      </c>
+      <c r="I19" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2916,10 +3045,16 @@
         <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>648</v>
+      </c>
+      <c r="H20" t="s">
+        <v>633</v>
+      </c>
+      <c r="I20" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2939,7 +3074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2956,10 +3091,16 @@
         <v>49</v>
       </c>
       <c r="F22" t="s">
+        <v>649</v>
+      </c>
+      <c r="H22" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2976,10 +3117,16 @@
         <v>51</v>
       </c>
       <c r="F23" t="s">
+        <v>650</v>
+      </c>
+      <c r="H23" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2999,7 +3146,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3019,7 +3166,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3039,7 +3186,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3059,7 +3206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3079,7 +3226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3099,7 +3246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3119,7 +3266,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3139,7 +3286,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5396,7 +5543,7 @@
         <v>8</v>
       </c>
       <c r="F144" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I144" t="s">
         <v>9</v>
@@ -5419,7 +5566,7 @@
         <v>10</v>
       </c>
       <c r="F145" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I145" t="s">
         <v>209</v>
@@ -5442,7 +5589,7 @@
         <v>210</v>
       </c>
       <c r="F146" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I146" t="s">
         <v>211</v>
@@ -5465,7 +5612,7 @@
         <v>14</v>
       </c>
       <c r="F147" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I147" t="s">
         <v>15</v>
@@ -5491,7 +5638,7 @@
         <v>17</v>
       </c>
       <c r="I148" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5882,7 +6029,7 @@
         <v>234</v>
       </c>
       <c r="F162" t="s">
-        <v>612</v>
+        <v>653</v>
       </c>
       <c r="G162" t="s">
         <v>590</v>
@@ -5911,7 +6058,7 @@
         <v>591</v>
       </c>
       <c r="F163" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G163" t="s">
         <v>596</v>
@@ -5940,7 +6087,7 @@
         <v>592</v>
       </c>
       <c r="F164" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G164" t="s">
         <v>597</v>
@@ -5969,7 +6116,7 @@
         <v>593</v>
       </c>
       <c r="F165" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G165" t="s">
         <v>598</v>
@@ -5978,7 +6125,7 @@
         <v>565</v>
       </c>
       <c r="I165" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5998,7 +6145,7 @@
         <v>594</v>
       </c>
       <c r="F166" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G166" t="s">
         <v>599</v>
@@ -6007,7 +6154,7 @@
         <v>565</v>
       </c>
       <c r="I166" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -6467,7 +6614,7 @@
         <v>241</v>
       </c>
       <c r="F189" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -8167,7 +8314,7 @@
         <v>192</v>
       </c>
       <c r="F274" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H274" t="s">
         <v>565</v>
@@ -8213,7 +8360,7 @@
         <v>196</v>
       </c>
       <c r="F276" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H276" t="s">
         <v>565</v>
@@ -8236,7 +8383,7 @@
         <v>198</v>
       </c>
       <c r="F277" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H277" t="s">
         <v>565</v>
@@ -8259,7 +8406,7 @@
         <v>200</v>
       </c>
       <c r="F278" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H278" t="s">
         <v>565</v>
@@ -8328,7 +8475,7 @@
         <v>206</v>
       </c>
       <c r="F281" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H281" t="s">
         <v>565</v>
@@ -12370,7 +12517,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E161" sqref="E161:E165"/>
+      <selection pane="bottomLeft" activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working on Caribou 1.3 analysis
</commit_message>
<xml_diff>
--- a/scripts/Provincial_Tools/tbl_sql_classify.xlsx
+++ b/scripts/Provincial_Tools/tbl_sql_classify.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1EB328-BD85-4007-8195-17A7EAB2DF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D80FB2-276F-4299-8B86-1A347256B6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="716">
   <si>
     <t>RECNO</t>
   </si>
@@ -2455,6 +2455,9 @@
   </si>
   <si>
     <t>originally EcoNum&gt;0</t>
+  </si>
+  <si>
+    <t>had chat with J. Mucha - HRDOM may need to move to POP?</t>
   </si>
 </sst>
 </file>
@@ -2838,7 +2841,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{78662066-8961-40A1-8222-90158F51F698}" name="Table2" displayName="Table2" ref="A1:I204" totalsRowShown="0">
-  <autoFilter ref="A1:I204" xr:uid="{78662066-8961-40A1-8222-90158F51F698}"/>
+  <autoFilter ref="A1:I204" xr:uid="{78662066-8961-40A1-8222-90158F51F698}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="PFT"/>
+        <filter val="SFU"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I204">
     <sortCondition ref="B2:B204"/>
     <sortCondition ref="C2:C204"/>
@@ -3178,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD4AE21-1701-4E7D-951A-9CFF25966ACE}">
   <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q97" sqref="Q97"/>
+    <sheetView tabSelected="1" topLeftCell="B122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I179" sqref="I179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,7 +3234,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>600</v>
       </c>
@@ -3244,7 +3254,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>601</v>
       </c>
@@ -3264,7 +3274,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>602</v>
       </c>
@@ -3284,7 +3294,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>603</v>
       </c>
@@ -3304,7 +3314,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>604</v>
       </c>
@@ -3327,7 +3337,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>810</v>
       </c>
@@ -3347,7 +3357,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>811</v>
       </c>
@@ -3367,7 +3377,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>812</v>
       </c>
@@ -3387,7 +3397,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>813</v>
       </c>
@@ -3407,7 +3417,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>814</v>
       </c>
@@ -3427,7 +3437,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>815</v>
       </c>
@@ -3447,7 +3457,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>816</v>
       </c>
@@ -3467,7 +3477,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>817</v>
       </c>
@@ -3487,7 +3497,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>680</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>681</v>
       </c>
@@ -3527,7 +3537,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>682</v>
       </c>
@@ -3547,7 +3557,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>683</v>
       </c>
@@ -3567,7 +3577,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>684</v>
       </c>
@@ -3587,7 +3597,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>805</v>
       </c>
@@ -3607,7 +3617,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>650</v>
       </c>
@@ -3627,7 +3637,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>651</v>
       </c>
@@ -3647,7 +3657,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>652</v>
       </c>
@@ -3667,7 +3677,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>653</v>
       </c>
@@ -3687,7 +3697,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>654</v>
       </c>
@@ -3707,7 +3717,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>655</v>
       </c>
@@ -3727,7 +3737,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>656</v>
       </c>
@@ -3747,7 +3757,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>657</v>
       </c>
@@ -3767,7 +3777,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>658</v>
       </c>
@@ -3787,7 +3797,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>659</v>
       </c>
@@ -3807,7 +3817,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>660</v>
       </c>
@@ -3827,7 +3837,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>661</v>
       </c>
@@ -3847,7 +3857,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>662</v>
       </c>
@@ -3867,7 +3877,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>663</v>
       </c>
@@ -3887,7 +3897,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>664</v>
       </c>
@@ -3907,7 +3917,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>665</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>666</v>
       </c>
@@ -3947,7 +3957,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>667</v>
       </c>
@@ -3967,7 +3977,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>668</v>
       </c>
@@ -3987,7 +3997,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>669</v>
       </c>
@@ -4007,7 +4017,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>670</v>
       </c>
@@ -4027,7 +4037,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>671</v>
       </c>
@@ -4047,7 +4057,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>672</v>
       </c>
@@ -4067,7 +4077,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>673</v>
       </c>
@@ -4087,7 +4097,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>674</v>
       </c>
@@ -4107,7 +4117,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>675</v>
       </c>
@@ -4127,7 +4137,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>676</v>
       </c>
@@ -4862,7 +4872,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>300</v>
       </c>
@@ -4885,7 +4895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>301</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>302</v>
       </c>
@@ -4931,7 +4941,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>303</v>
       </c>
@@ -4954,7 +4964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>304</v>
       </c>
@@ -4980,7 +4990,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>480</v>
       </c>
@@ -5000,7 +5010,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>481</v>
       </c>
@@ -5020,7 +5030,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>482</v>
       </c>
@@ -5040,7 +5050,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>483</v>
       </c>
@@ -5060,7 +5070,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>484</v>
       </c>
@@ -5080,7 +5090,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>485</v>
       </c>
@@ -5100,7 +5110,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>486</v>
       </c>
@@ -5120,7 +5130,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>487</v>
       </c>
@@ -5140,7 +5150,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>488</v>
       </c>
@@ -5160,7 +5170,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>442</v>
       </c>
@@ -5183,7 +5193,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>456</v>
       </c>
@@ -5206,7 +5216,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>400</v>
       </c>
@@ -5229,7 +5239,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>414</v>
       </c>
@@ -5252,7 +5262,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>428</v>
       </c>
@@ -5275,7 +5285,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>350</v>
       </c>
@@ -5298,7 +5308,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>351</v>
       </c>
@@ -5321,7 +5331,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>356</v>
       </c>
@@ -5344,7 +5354,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>359</v>
       </c>
@@ -5367,7 +5377,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>360</v>
       </c>
@@ -5390,7 +5400,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>362</v>
       </c>
@@ -5413,7 +5423,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>364</v>
       </c>
@@ -5436,7 +5446,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>365</v>
       </c>
@@ -5459,7 +5469,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>367</v>
       </c>
@@ -5482,7 +5492,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>208</v>
       </c>
@@ -5502,7 +5512,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>208</v>
       </c>
@@ -5522,7 +5532,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>208</v>
       </c>
@@ -5542,7 +5552,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>208</v>
       </c>
@@ -5562,7 +5572,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>208</v>
       </c>
@@ -6302,7 +6312,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1</v>
       </c>
@@ -6325,7 +6335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2</v>
       </c>
@@ -6348,7 +6358,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>3</v>
       </c>
@@ -6371,7 +6381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>4</v>
       </c>
@@ -6394,7 +6404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>5</v>
       </c>
@@ -6417,7 +6427,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>128</v>
       </c>
@@ -6437,7 +6447,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>129</v>
       </c>
@@ -6457,7 +6467,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>130</v>
       </c>
@@ -6477,7 +6487,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>131</v>
       </c>
@@ -6497,7 +6507,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>132</v>
       </c>
@@ -6517,7 +6527,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>133</v>
       </c>
@@ -6537,7 +6547,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>134</v>
       </c>
@@ -6557,7 +6567,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>6</v>
       </c>
@@ -6574,7 +6584,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>59</v>
       </c>
@@ -6594,7 +6604,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>75</v>
       </c>
@@ -6614,7 +6624,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>91</v>
       </c>
@@ -6634,7 +6644,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>107</v>
       </c>
@@ -6654,7 +6664,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>29</v>
       </c>
@@ -6674,7 +6684,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>30</v>
       </c>
@@ -6694,7 +6704,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>31</v>
       </c>
@@ -6714,7 +6724,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>32</v>
       </c>
@@ -6734,7 +6744,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>33</v>
       </c>
@@ -6754,7 +6764,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>34</v>
       </c>
@@ -6774,7 +6784,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>35</v>
       </c>
@@ -6794,7 +6804,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>36</v>
       </c>
@@ -6814,7 +6824,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>37</v>
       </c>
@@ -6834,7 +6844,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>38</v>
       </c>
@@ -6854,7 +6864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>39</v>
       </c>
@@ -6874,7 +6884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>40</v>
       </c>
@@ -6894,7 +6904,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>41</v>
       </c>
@@ -6914,7 +6924,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>42</v>
       </c>
@@ -7032,6 +7042,9 @@
       </c>
       <c r="F178" t="s">
         <v>201</v>
+      </c>
+      <c r="I178" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>